<commit_message>
Kedalion v.1.5 integracion opt+meltop+ked calculo manual y automatico lifeline base scraps
</commit_message>
<xml_diff>
--- a/Mix.xlsx
+++ b/Mix.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Documents\SIDER\Scrap Optimization\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5A12D74-6B97-4C80-A2F2-36594479059F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7428F0B9-870B-460A-A153-96D7B64D9BB3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="3396" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inventario" sheetId="9" r:id="rId1"/>
@@ -3103,6 +3103,12 @@
     <xf numFmtId="0" fontId="48" fillId="12" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="33" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="23" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3114,12 +3120,6 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -11235,8 +11235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C42D4128-7A49-4323-8F18-C858079FB1B4}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -11307,7 +11307,7 @@
         <v>0.32</v>
       </c>
       <c r="D2" s="229">
-        <v>6500</v>
+        <v>1700</v>
       </c>
       <c r="E2" s="229">
         <v>0</v>
@@ -11407,7 +11407,7 @@
         <v>0.43</v>
       </c>
       <c r="D4" s="229">
-        <v>17200</v>
+        <v>10000</v>
       </c>
       <c r="E4" s="229">
         <v>0</v>
@@ -11557,7 +11557,7 @@
         <v>1</v>
       </c>
       <c r="D7" s="229">
-        <v>9700</v>
+        <v>1000</v>
       </c>
       <c r="E7" s="229">
         <v>0</v>
@@ -11657,7 +11657,7 @@
         <v>0.6</v>
       </c>
       <c r="D9" s="229">
-        <v>4350</v>
+        <v>1200</v>
       </c>
       <c r="E9" s="229">
         <v>0</v>
@@ -12577,8 +12577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CF1F3EF-5E34-4FA8-A3D1-33686BE22993}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -12911,9 +12911,7 @@
       <c r="A17" s="159" t="s">
         <v>227</v>
       </c>
-      <c r="B17" s="229">
-        <v>0.2</v>
-      </c>
+      <c r="B17" s="229"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="234" t="s">
@@ -12925,25 +12923,19 @@
       <c r="A19" s="159" t="s">
         <v>228</v>
       </c>
-      <c r="B19" s="229">
-        <v>0.4</v>
-      </c>
+      <c r="B19" s="229"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="159" t="s">
         <v>229</v>
       </c>
-      <c r="B20" s="229">
-        <v>0.2</v>
-      </c>
+      <c r="B20" s="229"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="159" t="s">
         <v>230</v>
       </c>
-      <c r="B21" s="229">
-        <v>0.04</v>
-      </c>
+      <c r="B21" s="229"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -14218,7 +14210,7 @@
         <v>0.23194000000000001</v>
       </c>
       <c r="AB11" s="147">
-        <f t="shared" ref="AB11:AI11" si="14">SUMPRODUCT($B$2:$B$9,AB2:AB9)/$B$10</f>
+        <f t="shared" ref="AB11:AH11" si="14">SUMPRODUCT($B$2:$B$9,AB2:AB9)/$B$10</f>
         <v>0.53100000000000014</v>
       </c>
       <c r="AC11" s="147">
@@ -15251,10 +15243,10 @@
         <f>+B16+B27+B33+I19+B26+B38</f>
         <v>4757.4465272727284</v>
       </c>
-      <c r="N1" s="247" t="s">
+      <c r="N1" s="243" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="248"/>
+      <c r="O1" s="244"/>
       <c r="P1" s="64" t="s">
         <v>39</v>
       </c>
@@ -16374,7 +16366,7 @@
         <f>+K75</f>
         <v>0</v>
       </c>
-      <c r="D22" s="245" t="s">
+      <c r="D22" s="247" t="s">
         <v>231</v>
       </c>
       <c r="E22" s="69">
@@ -16417,7 +16409,7 @@
         <f>+I75</f>
         <v>16.380690000000001</v>
       </c>
-      <c r="D23" s="246"/>
+      <c r="D23" s="248"/>
       <c r="E23" s="71" t="s">
         <v>139</v>
       </c>
@@ -16603,7 +16595,7 @@
       <c r="B27" s="68">
         <v>0</v>
       </c>
-      <c r="D27" s="245" t="s">
+      <c r="D27" s="247" t="s">
         <v>50</v>
       </c>
       <c r="E27" s="69">
@@ -16656,7 +16648,7 @@
         <f>+B27*0.58+B26*0.86</f>
         <v>602</v>
       </c>
-      <c r="D28" s="246"/>
+      <c r="D28" s="248"/>
       <c r="E28" s="71" t="s">
         <v>139</v>
       </c>
@@ -18425,21 +18417,21 @@
       <c r="F78" s="56" t="s">
         <v>154</v>
       </c>
-      <c r="H78" s="243" t="s">
+      <c r="H78" s="245" t="s">
         <v>144</v>
       </c>
-      <c r="I78" s="243"/>
-      <c r="J78" s="243"/>
-      <c r="K78" s="243"/>
-      <c r="M78" s="243" t="s">
+      <c r="I78" s="245"/>
+      <c r="J78" s="245"/>
+      <c r="K78" s="245"/>
+      <c r="M78" s="245" t="s">
         <v>145</v>
       </c>
-      <c r="N78" s="243"/>
-      <c r="O78" s="243"/>
-      <c r="Q78" s="244" t="s">
+      <c r="N78" s="245"/>
+      <c r="O78" s="245"/>
+      <c r="Q78" s="246" t="s">
         <v>148</v>
       </c>
-      <c r="R78" s="244"/>
+      <c r="R78" s="246"/>
     </row>
     <row r="79" spans="1:18">
       <c r="A79" s="57" t="s">
@@ -18658,17 +18650,17 @@
       <c r="D90" s="98"/>
       <c r="E90" s="98"/>
       <c r="F90" s="98"/>
-      <c r="H90" s="243" t="s">
+      <c r="H90" s="245" t="s">
         <v>146</v>
       </c>
-      <c r="I90" s="243"/>
-      <c r="J90" s="243"/>
-      <c r="K90" s="243"/>
-      <c r="M90" s="243" t="s">
+      <c r="I90" s="245"/>
+      <c r="J90" s="245"/>
+      <c r="K90" s="245"/>
+      <c r="M90" s="245" t="s">
         <v>147</v>
       </c>
-      <c r="N90" s="243"/>
-      <c r="O90" s="243"/>
+      <c r="N90" s="245"/>
+      <c r="O90" s="245"/>
     </row>
     <row r="91" spans="1:15">
       <c r="B91" s="32">
@@ -19002,14 +18994,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="Q78:R78"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="D27:D28"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="H78:K78"/>
     <mergeCell ref="M78:O78"/>
     <mergeCell ref="H90:K90"/>
     <mergeCell ref="M90:O90"/>
-    <mergeCell ref="Q78:R78"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="D27:D28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -19067,10 +19059,10 @@
         <f>+B18+I15+I20+I25</f>
         <v>400.11745454545451</v>
       </c>
-      <c r="M2" s="247" t="s">
+      <c r="M2" s="243" t="s">
         <v>42</v>
       </c>
-      <c r="N2" s="248"/>
+      <c r="N2" s="244"/>
       <c r="O2" s="64" t="s">
         <v>39</v>
       </c>
@@ -19225,7 +19217,7 @@
       <c r="O7" s="32"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="D8" s="245" t="s">
+      <c r="D8" s="247" t="s">
         <v>50</v>
       </c>
       <c r="E8" s="69">
@@ -19262,7 +19254,7 @@
       <c r="A9" t="s">
         <v>173</v>
       </c>
-      <c r="D9" s="246"/>
+      <c r="D9" s="248"/>
       <c r="E9" s="71" t="s">
         <v>139</v>
       </c>
@@ -19455,10 +19447,10 @@
         <f>SUM(L16:L23)</f>
         <v>371.11302292119257</v>
       </c>
-      <c r="M15" s="247" t="s">
+      <c r="M15" s="243" t="s">
         <v>42</v>
       </c>
-      <c r="N15" s="248"/>
+      <c r="N15" s="244"/>
       <c r="O15" s="64" t="s">
         <v>39</v>
       </c>
@@ -21703,10 +21695,10 @@
         <f>+B16+B27+B33+I19+B26+B38</f>
         <v>4564.5246181818193</v>
       </c>
-      <c r="N1" s="247" t="s">
+      <c r="N1" s="243" t="s">
         <v>42</v>
       </c>
-      <c r="O1" s="248"/>
+      <c r="O1" s="244"/>
       <c r="P1" s="64" t="s">
         <v>39</v>
       </c>
@@ -22823,7 +22815,7 @@
         <f>+K78</f>
         <v>0</v>
       </c>
-      <c r="D22" s="245" t="s">
+      <c r="D22" s="247" t="s">
         <v>231</v>
       </c>
       <c r="E22" s="69">
@@ -22866,7 +22858,7 @@
         <f>+I78</f>
         <v>13.773177000000006</v>
       </c>
-      <c r="D23" s="246"/>
+      <c r="D23" s="248"/>
       <c r="E23" s="71" t="s">
         <v>139</v>
       </c>
@@ -23052,7 +23044,7 @@
       <c r="B27" s="68">
         <v>0</v>
       </c>
-      <c r="D27" s="245" t="s">
+      <c r="D27" s="247" t="s">
         <v>50</v>
       </c>
       <c r="E27" s="69">
@@ -23105,7 +23097,7 @@
         <f>+B27*0.58+B26*0.83</f>
         <v>581</v>
       </c>
-      <c r="D28" s="246"/>
+      <c r="D28" s="248"/>
       <c r="E28" s="71" t="s">
         <v>139</v>
       </c>
@@ -24873,21 +24865,21 @@
       <c r="F81" s="56" t="s">
         <v>154</v>
       </c>
-      <c r="H81" s="243" t="s">
+      <c r="H81" s="245" t="s">
         <v>144</v>
       </c>
-      <c r="I81" s="243"/>
-      <c r="J81" s="243"/>
-      <c r="K81" s="243"/>
-      <c r="M81" s="243" t="s">
+      <c r="I81" s="245"/>
+      <c r="J81" s="245"/>
+      <c r="K81" s="245"/>
+      <c r="M81" s="245" t="s">
         <v>145</v>
       </c>
-      <c r="N81" s="243"/>
-      <c r="O81" s="243"/>
-      <c r="Q81" s="244" t="s">
+      <c r="N81" s="245"/>
+      <c r="O81" s="245"/>
+      <c r="Q81" s="246" t="s">
         <v>148</v>
       </c>
-      <c r="R81" s="244"/>
+      <c r="R81" s="246"/>
     </row>
     <row r="82" spans="1:18">
       <c r="A82" s="57" t="s">
@@ -25106,17 +25098,17 @@
       <c r="D93" s="98"/>
       <c r="E93" s="98"/>
       <c r="F93" s="98"/>
-      <c r="H93" s="243" t="s">
+      <c r="H93" s="245" t="s">
         <v>146</v>
       </c>
-      <c r="I93" s="243"/>
-      <c r="J93" s="243"/>
-      <c r="K93" s="243"/>
-      <c r="M93" s="243" t="s">
+      <c r="I93" s="245"/>
+      <c r="J93" s="245"/>
+      <c r="K93" s="245"/>
+      <c r="M93" s="245" t="s">
         <v>147</v>
       </c>
-      <c r="N93" s="243"/>
-      <c r="O93" s="243"/>
+      <c r="N93" s="245"/>
+      <c r="O93" s="245"/>
     </row>
     <row r="94" spans="1:18">
       <c r="G94" s="36"/>

</xml_diff>